<commit_message>
first draft of retrieval evaluation
</commit_message>
<xml_diff>
--- a/exploration/esrs_datapoints.xlsx
+++ b/exploration/esrs_datapoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/zxowg46_s-cloud_uni-tuebingen_de/Documents/Thesis/esg_extraction/exploration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="865" documentId="13_ncr:1_{E347D4F0-AB2C-4238-BBDB-200313924039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AAA6C14-CC57-4CA6-BDB6-17811E32E3E0}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{276D0863-D6FD-4884-8A2A-6E3E35E67935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00A80B9F-830B-4093-BEDF-2002BF2B9F01}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="5" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2091" uniqueCount="756">
   <si>
     <t>List of ESRS Data Points</t>
   </si>
@@ -3413,6 +3413,18 @@
   </si>
   <si>
     <t>discrimination , harassment , equal opportunities, diversity , inclusion</t>
+  </si>
+  <si>
+    <t>grievance channels, raise concerns</t>
+  </si>
+  <si>
+    <t>engage, engagement, decision-making, representatives</t>
+  </si>
+  <si>
+    <t>dependencies, workforce risk, workforce opportunity, social risk, human capital, skill gap</t>
+  </si>
+  <si>
+    <t>postive impact</t>
   </si>
 </sst>
 </file>
@@ -3526,7 +3538,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3536,12 +3548,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3928,7 +3934,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="219">
+  <cellXfs count="217">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4296,9 +4302,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4431,100 +4434,99 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -4913,10 +4915,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5522,13 +5520,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C92534F0-4205-4B78-B15C-3308B949B405}">
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="139"/>
+    <col min="1" max="1" width="10.6640625" style="138"/>
     <col min="2" max="2" width="19.53125" style="136" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" style="133" customWidth="1"/>
     <col min="4" max="4" width="10.3984375" style="120" customWidth="1"/>
@@ -5544,7 +5542,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="129" customFormat="1" ht="94.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="138"/>
+      <c r="A1" s="137"/>
       <c r="B1" s="134" t="s">
         <v>288</v>
       </c>
@@ -5579,39 +5577,39 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="162" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="186" t="s">
+    <row r="2" spans="1:12" s="161" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="191" t="s">
         <v>702</v>
       </c>
-      <c r="B2" s="200" t="s">
+      <c r="B2" s="197" t="s">
         <v>701</v>
       </c>
-      <c r="C2" s="154" t="s">
+      <c r="C2" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="155" t="s">
+      <c r="D2" s="154" t="s">
         <v>96</v>
       </c>
-      <c r="E2" s="156" t="s">
+      <c r="E2" s="155" t="s">
         <v>97</v>
       </c>
-      <c r="F2" s="157" t="s">
+      <c r="F2" s="156" t="s">
         <v>654</v>
       </c>
-      <c r="G2" s="158"/>
-      <c r="H2" s="159" t="s">
-        <v>29</v>
-      </c>
-      <c r="I2" s="160"/>
-      <c r="J2" s="161"/>
-      <c r="K2" s="161" t="s">
+      <c r="G2" s="157"/>
+      <c r="H2" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="159"/>
+      <c r="J2" s="160"/>
+      <c r="K2" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L2" s="161"/>
+      <c r="L2" s="160"/>
     </row>
     <row r="3" spans="1:12" s="100" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="187"/>
-      <c r="B3" s="201"/>
+      <c r="A3" s="192"/>
+      <c r="B3" s="198"/>
       <c r="C3" s="132" t="s">
         <v>71</v>
       </c>
@@ -5638,8 +5636,8 @@
       <c r="L3" s="107"/>
     </row>
     <row r="4" spans="1:12" s="100" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="187"/>
-      <c r="B4" s="201"/>
+      <c r="A4" s="192"/>
+      <c r="B4" s="198"/>
       <c r="C4" s="132" t="s">
         <v>71</v>
       </c>
@@ -5663,65 +5661,65 @@
       </c>
       <c r="L4" s="107"/>
     </row>
-    <row r="5" spans="1:12" s="153" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="188"/>
-      <c r="B5" s="202"/>
-      <c r="C5" s="145" t="s">
+    <row r="5" spans="1:12" s="152" customFormat="1" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="193"/>
+      <c r="B5" s="199"/>
+      <c r="C5" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="146" t="s">
+      <c r="D5" s="145" t="s">
         <v>223</v>
       </c>
-      <c r="E5" s="147"/>
-      <c r="F5" s="148" t="s">
+      <c r="E5" s="146"/>
+      <c r="F5" s="147" t="s">
         <v>710</v>
       </c>
-      <c r="G5" s="149"/>
-      <c r="H5" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="151"/>
-      <c r="J5" s="152"/>
-      <c r="K5" s="152" t="s">
+      <c r="G5" s="148"/>
+      <c r="H5" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="150"/>
+      <c r="J5" s="151"/>
+      <c r="K5" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L5" s="152"/>
-    </row>
-    <row r="6" spans="1:12" s="164" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="186" t="s">
+      <c r="L5" s="151"/>
+    </row>
+    <row r="6" spans="1:12" s="163" customFormat="1" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="191" t="s">
         <v>704</v>
       </c>
-      <c r="B6" s="196" t="s">
+      <c r="B6" s="188" t="s">
         <v>289</v>
       </c>
-      <c r="C6" s="154" t="s">
+      <c r="C6" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D6" s="155">
+      <c r="D6" s="154">
         <v>14</v>
       </c>
-      <c r="E6" s="156" t="s">
+      <c r="E6" s="155" t="s">
         <v>85</v>
       </c>
-      <c r="F6" s="157" t="s">
+      <c r="F6" s="156" t="s">
         <v>650</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="162" t="s">
         <v>642</v>
       </c>
-      <c r="H6" s="164" t="s">
+      <c r="H6" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="162"/>
-      <c r="J6" s="161"/>
-      <c r="K6" s="161" t="s">
+      <c r="I6" s="161"/>
+      <c r="J6" s="160"/>
+      <c r="K6" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L6" s="161"/>
+      <c r="L6" s="160"/>
     </row>
     <row r="7" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="187"/>
-      <c r="B7" s="197"/>
+      <c r="A7" s="192"/>
+      <c r="B7" s="189"/>
       <c r="C7" s="132" t="s">
         <v>71</v>
       </c>
@@ -5744,8 +5742,8 @@
       <c r="L7" s="107"/>
     </row>
     <row r="8" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="187"/>
-      <c r="B8" s="197"/>
+      <c r="A8" s="192"/>
+      <c r="B8" s="189"/>
       <c r="C8" s="132" t="s">
         <v>71</v>
       </c>
@@ -5753,7 +5751,7 @@
         <v>100</v>
       </c>
       <c r="E8" s="108"/>
-      <c r="F8" s="191" t="s">
+      <c r="F8" s="196" t="s">
         <v>662</v>
       </c>
       <c r="G8" s="104" t="s">
@@ -5770,8 +5768,8 @@
       <c r="L8" s="107"/>
     </row>
     <row r="9" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="187"/>
-      <c r="B9" s="197"/>
+      <c r="A9" s="192"/>
+      <c r="B9" s="189"/>
       <c r="C9" s="132" t="s">
         <v>71</v>
       </c>
@@ -5779,7 +5777,7 @@
         <v>231</v>
       </c>
       <c r="E9" s="108"/>
-      <c r="F9" s="191"/>
+      <c r="F9" s="196"/>
       <c r="G9" s="104" t="s">
         <v>663</v>
       </c>
@@ -5795,67 +5793,67 @@
       </c>
       <c r="L9" s="107"/>
     </row>
-    <row r="10" spans="1:12" s="166" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="188"/>
-      <c r="B10" s="198"/>
-      <c r="C10" s="145" t="s">
+    <row r="10" spans="1:12" s="165" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="193"/>
+      <c r="B10" s="190"/>
+      <c r="C10" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D10" s="146">
+      <c r="D10" s="145">
         <v>43</v>
       </c>
-      <c r="E10" s="147"/>
-      <c r="F10" s="148" t="s">
+      <c r="E10" s="146"/>
+      <c r="F10" s="147" t="s">
         <v>660</v>
       </c>
-      <c r="G10" s="165" t="s">
+      <c r="G10" s="164" t="s">
         <v>661</v>
       </c>
-      <c r="H10" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="151"/>
-      <c r="J10" s="152"/>
-      <c r="K10" s="152" t="s">
+      <c r="H10" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I10" s="150"/>
+      <c r="J10" s="151"/>
+      <c r="K10" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L10" s="152"/>
-    </row>
-    <row r="11" spans="1:12" s="164" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="186" t="s">
+      <c r="L10" s="151"/>
+    </row>
+    <row r="11" spans="1:12" s="163" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="191" t="s">
         <v>705</v>
       </c>
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="188" t="s">
         <v>714</v>
       </c>
-      <c r="C11" s="154" t="s">
+      <c r="C11" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="155" t="s">
+      <c r="D11" s="154" t="s">
         <v>91</v>
       </c>
-      <c r="E11" s="167"/>
-      <c r="F11" s="157" t="s">
+      <c r="E11" s="166"/>
+      <c r="F11" s="156" t="s">
         <v>653</v>
       </c>
-      <c r="G11" s="168" t="s">
+      <c r="G11" s="167" t="s">
         <v>652</v>
       </c>
-      <c r="H11" s="164" t="s">
+      <c r="H11" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="169" t="s">
+      <c r="I11" s="168" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="161"/>
-      <c r="K11" s="161" t="s">
+      <c r="J11" s="160"/>
+      <c r="K11" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L11" s="161"/>
+      <c r="L11" s="160"/>
     </row>
     <row r="12" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="187"/>
-      <c r="B12" s="197"/>
+      <c r="A12" s="192"/>
+      <c r="B12" s="189"/>
       <c r="C12" s="132" t="s">
         <v>71</v>
       </c>
@@ -5880,8 +5878,8 @@
       <c r="L12" s="107"/>
     </row>
     <row r="13" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="187"/>
-      <c r="B13" s="197"/>
+      <c r="A13" s="192"/>
+      <c r="B13" s="189"/>
       <c r="C13" s="132" t="s">
         <v>71</v>
       </c>
@@ -5891,7 +5889,7 @@
       <c r="E13" s="102" t="s">
         <v>203</v>
       </c>
-      <c r="F13" s="195" t="s">
+      <c r="F13" s="204" t="s">
         <v>713</v>
       </c>
       <c r="G13" s="104"/>
@@ -5906,8 +5904,8 @@
       <c r="L13" s="107"/>
     </row>
     <row r="14" spans="1:12" ht="27.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="187"/>
-      <c r="B14" s="197"/>
+      <c r="A14" s="192"/>
+      <c r="B14" s="189"/>
       <c r="C14" s="132" t="s">
         <v>71</v>
       </c>
@@ -5917,7 +5915,7 @@
       <c r="E14" s="113" t="s">
         <v>213</v>
       </c>
-      <c r="F14" s="195"/>
+      <c r="F14" s="204"/>
       <c r="G14" s="104"/>
       <c r="H14" s="105" t="s">
         <v>29</v>
@@ -5930,8 +5928,8 @@
       <c r="L14" s="107"/>
     </row>
     <row r="15" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A15" s="187"/>
-      <c r="B15" s="197"/>
+      <c r="A15" s="192"/>
+      <c r="B15" s="189"/>
       <c r="C15" s="132" t="s">
         <v>71</v>
       </c>
@@ -5955,67 +5953,67 @@
       </c>
       <c r="L15" s="107"/>
     </row>
-    <row r="16" spans="1:12" s="166" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="188"/>
-      <c r="B16" s="198"/>
-      <c r="C16" s="145" t="s">
+    <row r="16" spans="1:12" s="165" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="193"/>
+      <c r="B16" s="190"/>
+      <c r="C16" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="146">
+      <c r="D16" s="145">
         <v>41</v>
       </c>
-      <c r="E16" s="170" t="s">
+      <c r="E16" s="169" t="s">
         <v>226</v>
       </c>
-      <c r="F16" s="148" t="s">
+      <c r="F16" s="147" t="s">
         <v>658</v>
       </c>
-      <c r="G16" s="149" t="s">
+      <c r="G16" s="148" t="s">
         <v>659</v>
       </c>
-      <c r="H16" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="151"/>
-      <c r="J16" s="152"/>
-      <c r="K16" s="152" t="s">
+      <c r="H16" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I16" s="150"/>
+      <c r="J16" s="151"/>
+      <c r="K16" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L16" s="152"/>
-    </row>
-    <row r="17" spans="1:12" s="164" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A17" s="186" t="s">
+      <c r="L16" s="151"/>
+    </row>
+    <row r="17" spans="1:12" s="163" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A17" s="191" t="s">
         <v>706</v>
       </c>
-      <c r="B17" s="196" t="s">
+      <c r="B17" s="188" t="s">
         <v>716</v>
       </c>
-      <c r="C17" s="154" t="s">
+      <c r="C17" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="155" t="s">
+      <c r="D17" s="154" t="s">
         <v>37</v>
       </c>
-      <c r="E17" s="167"/>
-      <c r="F17" s="157" t="s">
+      <c r="E17" s="166"/>
+      <c r="F17" s="156" t="s">
         <v>666</v>
       </c>
-      <c r="G17" s="158"/>
-      <c r="H17" s="159" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="160" t="s">
+      <c r="G17" s="157"/>
+      <c r="H17" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="159" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="161"/>
-      <c r="K17" s="161" t="s">
+      <c r="J17" s="160"/>
+      <c r="K17" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L17" s="161"/>
+      <c r="L17" s="160"/>
     </row>
     <row r="18" spans="1:12" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="187"/>
-      <c r="B18" s="197"/>
+      <c r="A18" s="192"/>
+      <c r="B18" s="189"/>
       <c r="C18" s="132" t="s">
         <v>71</v>
       </c>
@@ -6025,7 +6023,7 @@
       <c r="E18" s="102" t="s">
         <v>203</v>
       </c>
-      <c r="F18" s="191" t="s">
+      <c r="F18" s="196" t="s">
         <v>665</v>
       </c>
       <c r="G18" s="104"/>
@@ -6039,63 +6037,63 @@
       </c>
       <c r="L18" s="107"/>
     </row>
-    <row r="19" spans="1:12" s="166" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="188"/>
-      <c r="B19" s="198"/>
-      <c r="C19" s="145" t="s">
+    <row r="19" spans="1:12" s="165" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="193"/>
+      <c r="B19" s="190"/>
+      <c r="C19" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="171" t="s">
+      <c r="D19" s="170" t="s">
         <v>212</v>
       </c>
-      <c r="E19" s="172" t="s">
+      <c r="E19" s="171" t="s">
         <v>213</v>
       </c>
-      <c r="F19" s="199"/>
-      <c r="G19" s="149"/>
-      <c r="H19" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" s="151"/>
-      <c r="J19" s="152"/>
-      <c r="K19" s="152" t="s">
+      <c r="F19" s="200"/>
+      <c r="G19" s="148"/>
+      <c r="H19" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I19" s="150"/>
+      <c r="J19" s="151"/>
+      <c r="K19" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="152"/>
-    </row>
-    <row r="20" spans="1:12" s="164" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="186" t="s">
+      <c r="L19" s="151"/>
+    </row>
+    <row r="20" spans="1:12" s="163" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="191" t="s">
         <v>707</v>
       </c>
-      <c r="B20" s="192" t="s">
+      <c r="B20" s="201" t="s">
         <v>718</v>
       </c>
-      <c r="C20" s="154" t="s">
+      <c r="C20" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D20" s="174">
+      <c r="D20" s="173">
         <v>20</v>
       </c>
-      <c r="E20" s="167"/>
-      <c r="F20" s="157" t="s">
+      <c r="E20" s="166"/>
+      <c r="F20" s="156" t="s">
         <v>668</v>
       </c>
-      <c r="G20" s="158"/>
-      <c r="H20" s="159" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="160"/>
-      <c r="J20" s="161" t="s">
+      <c r="G20" s="157"/>
+      <c r="H20" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20" s="159"/>
+      <c r="J20" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K20" s="161" t="s">
+      <c r="K20" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L20" s="161"/>
+      <c r="L20" s="160"/>
     </row>
     <row r="21" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A21" s="187"/>
-      <c r="B21" s="193"/>
+      <c r="A21" s="192"/>
+      <c r="B21" s="202"/>
       <c r="C21" s="132" t="s">
         <v>71</v>
       </c>
@@ -6120,8 +6118,8 @@
       <c r="L21" s="107"/>
     </row>
     <row r="22" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="187"/>
-      <c r="B22" s="193"/>
+      <c r="A22" s="192"/>
+      <c r="B22" s="202"/>
       <c r="C22" s="132" t="s">
         <v>71</v>
       </c>
@@ -6148,8 +6146,8 @@
       <c r="L22" s="107"/>
     </row>
     <row r="23" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="187"/>
-      <c r="B23" s="193"/>
+      <c r="A23" s="192"/>
+      <c r="B23" s="202"/>
       <c r="C23" s="132" t="s">
         <v>71</v>
       </c>
@@ -6175,8 +6173,8 @@
       <c r="L23" s="107"/>
     </row>
     <row r="24" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="187"/>
-      <c r="B24" s="193"/>
+      <c r="A24" s="192"/>
+      <c r="B24" s="202"/>
       <c r="C24" s="132" t="s">
         <v>71</v>
       </c>
@@ -6201,8 +6199,8 @@
       <c r="L24" s="107"/>
     </row>
     <row r="25" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="187"/>
-      <c r="B25" s="193"/>
+      <c r="A25" s="192"/>
+      <c r="B25" s="202"/>
       <c r="C25" s="132" t="s">
         <v>71</v>
       </c>
@@ -6210,7 +6208,7 @@
         <v>103</v>
       </c>
       <c r="E25" s="108"/>
-      <c r="F25" s="191" t="s">
+      <c r="F25" s="196" t="s">
         <v>673</v>
       </c>
       <c r="G25" s="104"/>
@@ -6227,8 +6225,8 @@
       <c r="L25" s="107"/>
     </row>
     <row r="26" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="187"/>
-      <c r="B26" s="193"/>
+      <c r="A26" s="192"/>
+      <c r="B26" s="202"/>
       <c r="C26" s="132" t="s">
         <v>71</v>
       </c>
@@ -6236,7 +6234,7 @@
         <v>106</v>
       </c>
       <c r="E26" s="108"/>
-      <c r="F26" s="191"/>
+      <c r="F26" s="196"/>
       <c r="G26" s="104"/>
       <c r="H26" s="105" t="s">
         <v>29</v>
@@ -6251,8 +6249,8 @@
       <c r="L26" s="107"/>
     </row>
     <row r="27" spans="1:12" ht="26.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="187"/>
-      <c r="B27" s="193"/>
+      <c r="A27" s="192"/>
+      <c r="B27" s="202"/>
       <c r="C27" s="132" t="s">
         <v>71</v>
       </c>
@@ -6260,7 +6258,7 @@
         <v>109</v>
       </c>
       <c r="E27" s="108"/>
-      <c r="F27" s="191" t="s">
+      <c r="F27" s="196" t="s">
         <v>674</v>
       </c>
       <c r="G27" s="104"/>
@@ -6277,8 +6275,8 @@
       <c r="L27" s="107"/>
     </row>
     <row r="28" spans="1:12" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="187"/>
-      <c r="B28" s="193"/>
+      <c r="A28" s="192"/>
+      <c r="B28" s="202"/>
       <c r="C28" s="132" t="s">
         <v>71</v>
       </c>
@@ -6286,7 +6284,7 @@
         <v>112</v>
       </c>
       <c r="E28" s="108"/>
-      <c r="F28" s="191"/>
+      <c r="F28" s="196"/>
       <c r="G28" s="104"/>
       <c r="H28" s="105" t="s">
         <v>29</v>
@@ -6301,8 +6299,8 @@
       <c r="L28" s="107"/>
     </row>
     <row r="29" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="187"/>
-      <c r="B29" s="193"/>
+      <c r="A29" s="192"/>
+      <c r="B29" s="202"/>
       <c r="C29" s="132" t="s">
         <v>71</v>
       </c>
@@ -6325,97 +6323,97 @@
       </c>
       <c r="L29" s="107"/>
     </row>
-    <row r="30" spans="1:12" s="166" customFormat="1" ht="57.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A30" s="188"/>
-      <c r="B30" s="194"/>
-      <c r="C30" s="145" t="s">
+    <row r="30" spans="1:12" s="165" customFormat="1" ht="57.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A30" s="193"/>
+      <c r="B30" s="203"/>
+      <c r="C30" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D30" s="175" t="s">
+      <c r="D30" s="174" t="s">
         <v>166</v>
       </c>
-      <c r="E30" s="176" t="s">
+      <c r="E30" s="175" t="s">
         <v>167</v>
       </c>
-      <c r="F30" s="148" t="s">
+      <c r="F30" s="147" t="s">
         <v>685</v>
       </c>
-      <c r="G30" s="149"/>
-      <c r="H30" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="151" t="s">
+      <c r="G30" s="148"/>
+      <c r="H30" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="150" t="s">
         <v>30</v>
       </c>
-      <c r="J30" s="152"/>
-      <c r="K30" s="152" t="s">
+      <c r="J30" s="151"/>
+      <c r="K30" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L30" s="152"/>
-    </row>
-    <row r="31" spans="1:12" s="183" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="138" t="s">
+      <c r="L30" s="151"/>
+    </row>
+    <row r="31" spans="1:12" s="182" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A31" s="137" t="s">
         <v>708</v>
       </c>
-      <c r="B31" s="177" t="s">
+      <c r="B31" s="176" t="s">
         <v>725</v>
       </c>
-      <c r="C31" s="178" t="s">
+      <c r="C31" s="177" t="s">
         <v>71</v>
       </c>
-      <c r="D31" s="179">
+      <c r="D31" s="178">
         <v>23</v>
       </c>
-      <c r="E31" s="180"/>
-      <c r="F31" s="181" t="s">
+      <c r="E31" s="179"/>
+      <c r="F31" s="180" t="s">
         <v>671</v>
       </c>
-      <c r="G31" s="182"/>
-      <c r="H31" s="183" t="s">
+      <c r="G31" s="181"/>
+      <c r="H31" s="182" t="s">
         <v>28</v>
       </c>
       <c r="I31" s="129"/>
-      <c r="J31" s="184" t="s">
+      <c r="J31" s="183" t="s">
         <v>46</v>
       </c>
-      <c r="K31" s="184" t="s">
+      <c r="K31" s="183" t="s">
         <v>87</v>
       </c>
-      <c r="L31" s="184"/>
-    </row>
-    <row r="32" spans="1:12" s="164" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="186" t="s">
+      <c r="L31" s="183"/>
+    </row>
+    <row r="32" spans="1:12" s="163" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="191" t="s">
         <v>721</v>
       </c>
-      <c r="B32" s="196" t="s">
+      <c r="B32" s="188" t="s">
         <v>728</v>
       </c>
-      <c r="C32" s="154" t="s">
+      <c r="C32" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="174" t="s">
+      <c r="D32" s="173" t="s">
         <v>645</v>
       </c>
-      <c r="E32" s="167"/>
-      <c r="F32" s="157" t="s">
+      <c r="E32" s="166"/>
+      <c r="F32" s="156" t="s">
         <v>677</v>
       </c>
-      <c r="G32" s="168" t="s">
+      <c r="G32" s="167" t="s">
         <v>676</v>
       </c>
-      <c r="H32" s="164" t="s">
+      <c r="H32" s="163" t="s">
         <v>28</v>
       </c>
-      <c r="I32" s="162"/>
-      <c r="J32" s="161"/>
-      <c r="K32" s="161" t="s">
+      <c r="I32" s="161"/>
+      <c r="J32" s="160"/>
+      <c r="K32" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L32" s="161"/>
+      <c r="L32" s="160"/>
     </row>
     <row r="33" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A33" s="187"/>
-      <c r="B33" s="197"/>
+      <c r="A33" s="192"/>
+      <c r="B33" s="189"/>
       <c r="C33" s="132" t="s">
         <v>71</v>
       </c>
@@ -6442,8 +6440,8 @@
       <c r="L33" s="107"/>
     </row>
     <row r="34" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A34" s="187"/>
-      <c r="B34" s="197"/>
+      <c r="A34" s="192"/>
+      <c r="B34" s="189"/>
       <c r="C34" s="132" t="s">
         <v>71</v>
       </c>
@@ -6465,63 +6463,63 @@
       </c>
       <c r="L34" s="107"/>
     </row>
-    <row r="35" spans="1:12" s="166" customFormat="1" ht="71.650000000000006" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="188"/>
-      <c r="B35" s="198"/>
-      <c r="C35" s="145" t="s">
+    <row r="35" spans="1:12" s="165" customFormat="1" ht="71.650000000000006" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A35" s="193"/>
+      <c r="B35" s="190"/>
+      <c r="C35" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="175" t="s">
+      <c r="D35" s="174" t="s">
         <v>648</v>
       </c>
-      <c r="E35" s="147"/>
-      <c r="F35" s="148" t="s">
+      <c r="E35" s="146"/>
+      <c r="F35" s="147" t="s">
         <v>681</v>
       </c>
-      <c r="G35" s="149"/>
-      <c r="H35" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I35" s="151"/>
-      <c r="J35" s="152"/>
-      <c r="K35" s="152" t="s">
+      <c r="G35" s="148"/>
+      <c r="H35" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I35" s="150"/>
+      <c r="J35" s="151"/>
+      <c r="K35" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L35" s="152"/>
-    </row>
-    <row r="36" spans="1:12" s="164" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="186" t="s">
+      <c r="L35" s="151"/>
+    </row>
+    <row r="36" spans="1:12" s="163" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="191" t="s">
         <v>722</v>
       </c>
-      <c r="B36" s="196" t="s">
+      <c r="B36" s="188" t="s">
         <v>682</v>
       </c>
-      <c r="C36" s="154" t="s">
+      <c r="C36" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D36" s="174" t="s">
+      <c r="D36" s="173" t="s">
         <v>126</v>
       </c>
-      <c r="E36" s="167"/>
-      <c r="F36" s="157" t="s">
+      <c r="E36" s="166"/>
+      <c r="F36" s="156" t="s">
         <v>683</v>
       </c>
-      <c r="G36" s="158"/>
-      <c r="H36" s="159" t="s">
-        <v>29</v>
-      </c>
-      <c r="I36" s="160"/>
-      <c r="J36" s="161" t="s">
+      <c r="G36" s="157"/>
+      <c r="H36" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I36" s="159"/>
+      <c r="J36" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K36" s="161" t="s">
+      <c r="K36" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L36" s="161"/>
+      <c r="L36" s="160"/>
     </row>
     <row r="37" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A37" s="187"/>
-      <c r="B37" s="197"/>
+      <c r="A37" s="192"/>
+      <c r="B37" s="189"/>
       <c r="C37" s="132" t="s">
         <v>71</v>
       </c>
@@ -6546,8 +6544,8 @@
       <c r="L37" s="107"/>
     </row>
     <row r="38" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A38" s="187"/>
-      <c r="B38" s="197"/>
+      <c r="A38" s="192"/>
+      <c r="B38" s="189"/>
       <c r="C38" s="132" t="s">
         <v>71</v>
       </c>
@@ -6571,8 +6569,8 @@
       <c r="L38" s="107"/>
     </row>
     <row r="39" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="187"/>
-      <c r="B39" s="197"/>
+      <c r="A39" s="192"/>
+      <c r="B39" s="189"/>
       <c r="C39" s="132" t="s">
         <v>71</v>
       </c>
@@ -6599,8 +6597,8 @@
       <c r="L39" s="107"/>
     </row>
     <row r="40" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A40" s="187"/>
-      <c r="B40" s="197"/>
+      <c r="A40" s="192"/>
+      <c r="B40" s="189"/>
       <c r="C40" s="132" t="s">
         <v>71</v>
       </c>
@@ -6627,8 +6625,8 @@
       <c r="L40" s="107"/>
     </row>
     <row r="41" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="187"/>
-      <c r="B41" s="197"/>
+      <c r="A41" s="192"/>
+      <c r="B41" s="189"/>
       <c r="C41" s="132" t="s">
         <v>71</v>
       </c>
@@ -6653,8 +6651,8 @@
       <c r="L41" s="107"/>
     </row>
     <row r="42" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A42" s="187"/>
-      <c r="B42" s="197"/>
+      <c r="A42" s="192"/>
+      <c r="B42" s="189"/>
       <c r="C42" s="132" t="s">
         <v>71</v>
       </c>
@@ -6679,8 +6677,8 @@
       <c r="L42" s="107"/>
     </row>
     <row r="43" spans="1:12" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="187"/>
-      <c r="B43" s="197"/>
+      <c r="A43" s="192"/>
+      <c r="B43" s="189"/>
       <c r="C43" s="132" t="s">
         <v>71</v>
       </c>
@@ -6688,7 +6686,7 @@
         <v>235</v>
       </c>
       <c r="E43" s="108"/>
-      <c r="F43" s="191" t="s">
+      <c r="F43" s="196" t="s">
         <v>732</v>
       </c>
       <c r="G43" s="104"/>
@@ -6703,8 +6701,8 @@
       <c r="L43" s="107"/>
     </row>
     <row r="44" spans="1:12" ht="27" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="187"/>
-      <c r="B44" s="197"/>
+      <c r="A44" s="192"/>
+      <c r="B44" s="189"/>
       <c r="C44" s="132" t="s">
         <v>71</v>
       </c>
@@ -6712,7 +6710,7 @@
         <v>238</v>
       </c>
       <c r="E44" s="108"/>
-      <c r="F44" s="191"/>
+      <c r="F44" s="196"/>
       <c r="G44" s="104"/>
       <c r="H44" s="105" t="s">
         <v>29</v>
@@ -6724,61 +6722,61 @@
       </c>
       <c r="L44" s="107"/>
     </row>
-    <row r="45" spans="1:12" s="166" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="188"/>
-      <c r="B45" s="198"/>
-      <c r="C45" s="145" t="s">
+    <row r="45" spans="1:12" s="165" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A45" s="193"/>
+      <c r="B45" s="190"/>
+      <c r="C45" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D45" s="146" t="s">
+      <c r="D45" s="145" t="s">
         <v>241</v>
       </c>
-      <c r="E45" s="147"/>
-      <c r="F45" s="199"/>
-      <c r="G45" s="149"/>
-      <c r="H45" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I45" s="151"/>
-      <c r="J45" s="152"/>
-      <c r="K45" s="152" t="s">
+      <c r="E45" s="146"/>
+      <c r="F45" s="200"/>
+      <c r="G45" s="148"/>
+      <c r="H45" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="150"/>
+      <c r="J45" s="151"/>
+      <c r="K45" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L45" s="152"/>
-    </row>
-    <row r="46" spans="1:12" s="164" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A46" s="186" t="s">
+      <c r="L45" s="151"/>
+    </row>
+    <row r="46" spans="1:12" s="163" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A46" s="191" t="s">
         <v>723</v>
       </c>
-      <c r="B46" s="196" t="s">
+      <c r="B46" s="188" t="s">
         <v>736</v>
       </c>
-      <c r="C46" s="154" t="s">
+      <c r="C46" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="174" t="s">
+      <c r="D46" s="173" t="s">
         <v>129</v>
       </c>
-      <c r="E46" s="167"/>
-      <c r="F46" s="157" t="s">
+      <c r="E46" s="166"/>
+      <c r="F46" s="156" t="s">
         <v>688</v>
       </c>
-      <c r="G46" s="158"/>
-      <c r="H46" s="159" t="s">
-        <v>29</v>
-      </c>
-      <c r="I46" s="160"/>
-      <c r="J46" s="161" t="s">
+      <c r="G46" s="157"/>
+      <c r="H46" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="159"/>
+      <c r="J46" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="K46" s="161" t="s">
+      <c r="K46" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L46" s="161"/>
+      <c r="L46" s="160"/>
     </row>
     <row r="47" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A47" s="187"/>
-      <c r="B47" s="197"/>
+      <c r="A47" s="192"/>
+      <c r="B47" s="189"/>
       <c r="C47" s="132" t="s">
         <v>71</v>
       </c>
@@ -6802,63 +6800,63 @@
       </c>
       <c r="L47" s="107"/>
     </row>
-    <row r="48" spans="1:12" s="166" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A48" s="188"/>
-      <c r="B48" s="198"/>
-      <c r="C48" s="145" t="s">
+    <row r="48" spans="1:12" s="165" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A48" s="193"/>
+      <c r="B48" s="190"/>
+      <c r="C48" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D48" s="146" t="s">
+      <c r="D48" s="145" t="s">
         <v>206</v>
       </c>
-      <c r="E48" s="147"/>
-      <c r="F48" s="148" t="s">
+      <c r="E48" s="146"/>
+      <c r="F48" s="147" t="s">
         <v>690</v>
       </c>
-      <c r="G48" s="149"/>
-      <c r="H48" s="150" t="s">
-        <v>29</v>
-      </c>
-      <c r="I48" s="151"/>
-      <c r="J48" s="152"/>
-      <c r="K48" s="152" t="s">
+      <c r="G48" s="148"/>
+      <c r="H48" s="149" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="150"/>
+      <c r="J48" s="151"/>
+      <c r="K48" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L48" s="152"/>
-    </row>
-    <row r="49" spans="1:12" s="164" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A49" s="186" t="s">
+      <c r="L48" s="151"/>
+    </row>
+    <row r="49" spans="1:12" s="163" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A49" s="191" t="s">
         <v>724</v>
       </c>
-      <c r="B49" s="196" t="s">
+      <c r="B49" s="188" t="s">
         <v>738</v>
       </c>
-      <c r="C49" s="154" t="s">
+      <c r="C49" s="153" t="s">
         <v>71</v>
       </c>
-      <c r="D49" s="174" t="s">
+      <c r="D49" s="173" t="s">
         <v>180</v>
       </c>
-      <c r="E49" s="156" t="s">
+      <c r="E49" s="155" t="s">
         <v>181</v>
       </c>
-      <c r="F49" s="157" t="s">
+      <c r="F49" s="156" t="s">
         <v>691</v>
       </c>
-      <c r="G49" s="158"/>
-      <c r="H49" s="159" t="s">
-        <v>29</v>
-      </c>
-      <c r="I49" s="160"/>
-      <c r="J49" s="161"/>
-      <c r="K49" s="161" t="s">
+      <c r="G49" s="157"/>
+      <c r="H49" s="158" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="159"/>
+      <c r="J49" s="160"/>
+      <c r="K49" s="160" t="s">
         <v>87</v>
       </c>
-      <c r="L49" s="161"/>
+      <c r="L49" s="160"/>
     </row>
     <row r="50" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="187"/>
-      <c r="B50" s="197"/>
+      <c r="A50" s="192"/>
+      <c r="B50" s="189"/>
       <c r="C50" s="132" t="s">
         <v>71</v>
       </c>
@@ -6882,8 +6880,8 @@
       <c r="L50" s="107"/>
     </row>
     <row r="51" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A51" s="187"/>
-      <c r="B51" s="197"/>
+      <c r="A51" s="192"/>
+      <c r="B51" s="189"/>
       <c r="C51" s="132" t="s">
         <v>71</v>
       </c>
@@ -6906,8 +6904,8 @@
       <c r="L51" s="107"/>
     </row>
     <row r="52" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A52" s="187"/>
-      <c r="B52" s="197"/>
+      <c r="A52" s="192"/>
+      <c r="B52" s="189"/>
       <c r="C52" s="132" t="s">
         <v>71</v>
       </c>
@@ -6932,8 +6930,8 @@
       <c r="L52" s="107"/>
     </row>
     <row r="53" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A53" s="187"/>
-      <c r="B53" s="197"/>
+      <c r="A53" s="192"/>
+      <c r="B53" s="189"/>
       <c r="C53" s="132" t="s">
         <v>71</v>
       </c>
@@ -6957,37 +6955,37 @@
       </c>
       <c r="L53" s="107"/>
     </row>
-    <row r="54" spans="1:12" s="166" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A54" s="188"/>
-      <c r="B54" s="198"/>
-      <c r="C54" s="145" t="s">
+    <row r="54" spans="1:12" s="165" customFormat="1" ht="43.15" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A54" s="193"/>
+      <c r="B54" s="190"/>
+      <c r="C54" s="144" t="s">
         <v>71</v>
       </c>
-      <c r="D54" s="175">
+      <c r="D54" s="174">
         <v>33</v>
       </c>
-      <c r="E54" s="147"/>
-      <c r="F54" s="148" t="s">
+      <c r="E54" s="146"/>
+      <c r="F54" s="147" t="s">
         <v>696</v>
       </c>
-      <c r="G54" s="165"/>
-      <c r="H54" s="166" t="s">
+      <c r="G54" s="164"/>
+      <c r="H54" s="165" t="s">
         <v>28</v>
       </c>
-      <c r="I54" s="185" t="s">
+      <c r="I54" s="184" t="s">
         <v>30</v>
       </c>
-      <c r="J54" s="152"/>
-      <c r="K54" s="152" t="s">
+      <c r="J54" s="151"/>
+      <c r="K54" s="151" t="s">
         <v>87</v>
       </c>
-      <c r="L54" s="152"/>
-    </row>
-    <row r="55" spans="1:12" s="144" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A55" s="140" t="s">
+      <c r="L54" s="151"/>
+    </row>
+    <row r="55" spans="1:12" s="143" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A55" s="139" t="s">
         <v>734</v>
       </c>
-      <c r="B55" s="173" t="s">
+      <c r="B55" s="172" t="s">
         <v>742</v>
       </c>
       <c r="C55" s="131" t="s">
@@ -7002,8 +7000,8 @@
       <c r="F55" s="122" t="s">
         <v>697</v>
       </c>
-      <c r="G55" s="143"/>
-      <c r="H55" s="144" t="s">
+      <c r="G55" s="142"/>
+      <c r="H55" s="143" t="s">
         <v>28</v>
       </c>
       <c r="I55" s="124"/>
@@ -7014,10 +7012,10 @@
       <c r="L55" s="123"/>
     </row>
     <row r="56" spans="1:12" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A56" s="189" t="s">
+      <c r="A56" s="194" t="s">
         <v>735</v>
       </c>
-      <c r="B56" s="197" t="s">
+      <c r="B56" s="189" t="s">
         <v>744</v>
       </c>
       <c r="C56" s="132" t="s">
@@ -7029,7 +7027,7 @@
       <c r="E56" s="102" t="s">
         <v>250</v>
       </c>
-      <c r="F56" s="191" t="s">
+      <c r="F56" s="196" t="s">
         <v>699</v>
       </c>
       <c r="G56" s="116" t="s">
@@ -7048,8 +7046,8 @@
       </c>
     </row>
     <row r="57" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A57" s="187"/>
-      <c r="B57" s="197"/>
+      <c r="A57" s="192"/>
+      <c r="B57" s="189"/>
       <c r="C57" s="132" t="s">
         <v>71</v>
       </c>
@@ -7059,7 +7057,7 @@
       <c r="E57" s="102" t="s">
         <v>250</v>
       </c>
-      <c r="F57" s="191"/>
+      <c r="F57" s="196"/>
       <c r="G57" s="119"/>
       <c r="H57" s="117" t="s">
         <v>28</v>
@@ -7074,8 +7072,8 @@
       </c>
     </row>
     <row r="58" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="187"/>
-      <c r="B58" s="197"/>
+      <c r="A58" s="192"/>
+      <c r="B58" s="189"/>
       <c r="C58" s="132" t="s">
         <v>71</v>
       </c>
@@ -7085,7 +7083,7 @@
       <c r="E58" s="102" t="s">
         <v>250</v>
       </c>
-      <c r="F58" s="191"/>
+      <c r="F58" s="196"/>
       <c r="G58" s="119"/>
       <c r="H58" s="117" t="s">
         <v>28</v>
@@ -7100,8 +7098,8 @@
       </c>
     </row>
     <row r="59" spans="1:12" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A59" s="187"/>
-      <c r="B59" s="197"/>
+      <c r="A59" s="192"/>
+      <c r="B59" s="189"/>
       <c r="C59" s="132" t="s">
         <v>71</v>
       </c>
@@ -7111,7 +7109,7 @@
       <c r="E59" s="102" t="s">
         <v>250</v>
       </c>
-      <c r="F59" s="191"/>
+      <c r="F59" s="196"/>
       <c r="G59" s="119"/>
       <c r="H59" s="117" t="s">
         <v>28</v>
@@ -7126,8 +7124,8 @@
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A60" s="187"/>
-      <c r="B60" s="197"/>
+      <c r="A60" s="192"/>
+      <c r="B60" s="189"/>
       <c r="C60" s="132" t="s">
         <v>71</v>
       </c>
@@ -7137,7 +7135,7 @@
       <c r="E60" s="102" t="s">
         <v>250</v>
       </c>
-      <c r="F60" s="191"/>
+      <c r="F60" s="196"/>
       <c r="G60" s="119"/>
       <c r="H60" s="117" t="s">
         <v>28</v>
@@ -7152,8 +7150,8 @@
       </c>
     </row>
     <row r="61" spans="1:12" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A61" s="190"/>
-      <c r="B61" s="197"/>
+      <c r="A61" s="195"/>
+      <c r="B61" s="189"/>
       <c r="C61" s="132" t="s">
         <v>71</v>
       </c>
@@ -7184,33 +7182,33 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="B6:B10"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="F56:F60"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="B56:B61"/>
+    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="B2:B5"/>
     <mergeCell ref="B36:B45"/>
     <mergeCell ref="F25:F26"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="F43:F45"/>
     <mergeCell ref="B32:B35"/>
+    <mergeCell ref="B20:B30"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="B6:B10"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="B11:B16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="B20:B30"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A20:A30"/>
-    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="A36:A45"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A49:A54"/>
     <mergeCell ref="A56:A61"/>
-    <mergeCell ref="F56:F60"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="B56:B61"/>
-    <mergeCell ref="B49:B54"/>
+    <mergeCell ref="A32:A35"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="D2:D13 D15:D18 D20:D28 D30:D54 D56:D60">
@@ -7323,8 +7321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B442CA99-AF6D-4997-8E84-42BB9E92AEF4}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7336,47 +7334,50 @@
     <col min="6" max="6" width="56.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="141" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="B1" s="142" t="s">
+    <row r="1" spans="1:6" s="140" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B1" s="141" t="s">
         <v>288</v>
       </c>
-      <c r="C1" s="142" t="s">
+      <c r="C1" s="141" t="s">
         <v>712</v>
       </c>
-      <c r="F1" s="141" t="s">
+      <c r="F1" s="140" t="s">
         <v>746</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" s="185" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="185" t="s">
         <v>702</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="186" t="s">
         <v>701</v>
       </c>
-      <c r="C2" s="137" t="s">
+      <c r="C2" s="187" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+      <c r="F2" s="185" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="185" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="185" t="s">
         <v>704</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="186" t="s">
         <v>289</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="186" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" s="185" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="185" t="s">
         <v>705</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="186" t="s">
         <v>714</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="186" t="s">
         <v>715</v>
       </c>
     </row>
@@ -7390,116 +7391,125 @@
       <c r="C5" s="2" t="s">
         <v>717</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" s="217" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="217" t="s">
+      <c r="F5" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="185" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="185" t="s">
         <v>707</v>
       </c>
-      <c r="B6" s="218" t="s">
+      <c r="B6" s="186" t="s">
         <v>718</v>
       </c>
-      <c r="C6" s="218" t="s">
+      <c r="C6" s="186" t="s">
         <v>719</v>
       </c>
-      <c r="F6" s="217" t="s">
+      <c r="F6" s="185" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="217" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="217" t="s">
+    <row r="7" spans="1:6" s="185" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="185" t="s">
         <v>708</v>
       </c>
-      <c r="B7" s="218" t="s">
+      <c r="B7" s="186" t="s">
         <v>725</v>
       </c>
-      <c r="C7" s="218" t="s">
+      <c r="C7" s="186" t="s">
         <v>720</v>
       </c>
-      <c r="F7" s="218" t="s">
+      <c r="F7" s="186" t="s">
         <v>747</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="217" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A8" s="217" t="s">
+    <row r="8" spans="1:6" s="185" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A8" s="185" t="s">
         <v>721</v>
       </c>
-      <c r="B8" s="218" t="s">
+      <c r="B8" s="186" t="s">
         <v>728</v>
       </c>
-      <c r="C8" s="218" t="s">
+      <c r="C8" s="186" t="s">
         <v>726</v>
       </c>
-      <c r="D8" s="218" t="s">
+      <c r="D8" s="186" t="s">
         <v>727</v>
       </c>
-      <c r="F8" s="217" t="s">
+      <c r="F8" s="185" t="s">
         <v>751</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" s="185" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="185" t="s">
         <v>722</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="186" t="s">
         <v>682</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="186" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="217" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="217" t="s">
+      <c r="F9" s="185" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="185" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A10" s="185" t="s">
         <v>723</v>
       </c>
-      <c r="B10" s="218" t="s">
+      <c r="B10" s="186" t="s">
         <v>736</v>
       </c>
-      <c r="C10" s="218" t="s">
+      <c r="C10" s="186" t="s">
         <v>737</v>
       </c>
-      <c r="F10" s="217" t="s">
+      <c r="F10" s="185" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="215" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="215" t="s">
+    <row r="11" spans="1:6" s="185" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="185" t="s">
         <v>724</v>
       </c>
-      <c r="B11" s="216" t="s">
+      <c r="B11" s="186" t="s">
         <v>738</v>
       </c>
-      <c r="C11" s="216" t="s">
+      <c r="C11" s="186" t="s">
         <v>740</v>
       </c>
-      <c r="D11" s="216" t="s">
+      <c r="D11" s="186" t="s">
         <v>739</v>
       </c>
-      <c r="E11" s="216" t="s">
+      <c r="E11" s="186" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" s="217" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="217" t="s">
+      <c r="F11" s="185" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="185" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A12" s="185" t="s">
         <v>734</v>
       </c>
-      <c r="B12" s="218" t="s">
+      <c r="B12" s="186" t="s">
         <v>742</v>
       </c>
-      <c r="C12" s="218" t="s">
+      <c r="C12" s="186" t="s">
         <v>745</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="217" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A13" s="217" t="s">
+    <row r="13" spans="1:6" s="185" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="A13" s="185" t="s">
         <v>735</v>
       </c>
-      <c r="B13" s="218" t="s">
+      <c r="B13" s="186" t="s">
         <v>744</v>
       </c>
-      <c r="C13" s="218" t="s">
+      <c r="C13" s="186" t="s">
         <v>743</v>
       </c>
-      <c r="F13" s="217" t="s">
+      <c r="F13" s="185" t="s">
         <v>750</v>
       </c>
     </row>
@@ -7512,7 +7522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612EC7FB-07B4-4895-8A1B-BC9CDD0AE99E}">
   <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
@@ -7572,7 +7582,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="32.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="203" t="s">
+      <c r="A2" s="205" t="s">
         <v>289</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -7605,7 +7615,7 @@
       <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="204"/>
+      <c r="A3" s="206"/>
       <c r="B3" s="3" t="s">
         <v>88</v>
       </c>
@@ -7634,7 +7644,7 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="204"/>
+      <c r="A4" s="206"/>
       <c r="B4" s="3" t="s">
         <v>95</v>
       </c>
@@ -7665,7 +7675,7 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="204"/>
+      <c r="A5" s="206"/>
       <c r="B5" s="3" t="s">
         <v>99</v>
       </c>
@@ -7694,7 +7704,7 @@
       <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="204"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="3" t="s">
         <v>117</v>
       </c>
@@ -7725,7 +7735,7 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="204"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="3" t="s">
         <v>218</v>
       </c>
@@ -7756,7 +7766,7 @@
       <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="205"/>
+      <c r="A8" s="207"/>
       <c r="B8" s="3" t="s">
         <v>222</v>
       </c>
@@ -7785,7 +7795,7 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13" s="44" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="203" t="s">
+      <c r="A9" s="205" t="s">
         <v>296</v>
       </c>
       <c r="B9" s="38" t="s">
@@ -7818,7 +7828,7 @@
       <c r="M9" s="43"/>
     </row>
     <row r="10" spans="1:13" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="204"/>
+      <c r="A10" s="206"/>
       <c r="B10" s="3" t="s">
         <v>114</v>
       </c>
@@ -7849,7 +7859,7 @@
       <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" ht="46.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="204"/>
+      <c r="A11" s="206"/>
       <c r="B11" s="3" t="s">
         <v>201</v>
       </c>
@@ -7880,7 +7890,7 @@
       <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="204"/>
+      <c r="A12" s="206"/>
       <c r="B12" s="3" t="s">
         <v>211</v>
       </c>
@@ -7911,7 +7921,7 @@
       <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="204"/>
+      <c r="A13" s="206"/>
       <c r="B13" s="3" t="s">
         <v>215</v>
       </c>
@@ -7942,7 +7952,7 @@
       <c r="M13" s="16"/>
     </row>
     <row r="14" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="204"/>
+      <c r="A14" s="206"/>
       <c r="B14" s="3" t="s">
         <v>225</v>
       </c>
@@ -7973,7 +7983,7 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A15" s="204"/>
+      <c r="A15" s="206"/>
       <c r="B15" s="3" t="s">
         <v>228</v>
       </c>
@@ -8002,7 +8012,7 @@
       <c r="M15" s="16"/>
     </row>
     <row r="16" spans="1:13" s="29" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A16" s="205"/>
+      <c r="A16" s="207"/>
       <c r="B16" s="30" t="s">
         <v>230</v>
       </c>
@@ -8033,7 +8043,7 @@
       <c r="M16" s="35"/>
     </row>
     <row r="17" spans="1:13" s="44" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="203" t="s">
+      <c r="A17" s="205" t="s">
         <v>297</v>
       </c>
       <c r="B17" s="38" t="s">
@@ -8066,7 +8076,7 @@
       <c r="M17" s="43"/>
     </row>
     <row r="18" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="204"/>
+      <c r="A18" s="206"/>
       <c r="B18" s="3" t="s">
         <v>208</v>
       </c>
@@ -8097,7 +8107,7 @@
       <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="205"/>
+      <c r="A19" s="207"/>
       <c r="B19" s="3" t="s">
         <v>211</v>
       </c>
@@ -8128,7 +8138,7 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" s="44" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="203" t="s">
+      <c r="A20" s="205" t="s">
         <v>294</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -8161,7 +8171,7 @@
       <c r="M20" s="43"/>
     </row>
     <row r="21" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A21" s="204"/>
+      <c r="A21" s="206"/>
       <c r="B21" s="3" t="s">
         <v>122</v>
       </c>
@@ -8192,7 +8202,7 @@
       <c r="M21" s="16"/>
     </row>
     <row r="22" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="204"/>
+      <c r="A22" s="206"/>
       <c r="B22" s="3" t="s">
         <v>125</v>
       </c>
@@ -8223,7 +8233,7 @@
       <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="204"/>
+      <c r="A23" s="206"/>
       <c r="B23" s="3" t="s">
         <v>128</v>
       </c>
@@ -8254,7 +8264,7 @@
       <c r="M23" s="16"/>
     </row>
     <row r="24" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="204"/>
+      <c r="A24" s="206"/>
       <c r="B24" s="3" t="s">
         <v>131</v>
       </c>
@@ -8287,7 +8297,7 @@
       <c r="M24" s="16"/>
     </row>
     <row r="25" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="204"/>
+      <c r="A25" s="206"/>
       <c r="B25" s="3" t="s">
         <v>276</v>
       </c>
@@ -8320,7 +8330,7 @@
       <c r="M25" s="16"/>
     </row>
     <row r="26" spans="1:13" s="29" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A26" s="205"/>
+      <c r="A26" s="207"/>
       <c r="B26" s="30" t="s">
         <v>280</v>
       </c>
@@ -8351,7 +8361,7 @@
       <c r="M26" s="35"/>
     </row>
     <row r="27" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="204" t="s">
+      <c r="A27" s="206" t="s">
         <v>292</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -8384,7 +8394,7 @@
       <c r="M27" s="16"/>
     </row>
     <row r="28" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A28" s="204"/>
+      <c r="A28" s="206"/>
       <c r="B28" s="3" t="s">
         <v>105</v>
       </c>
@@ -8415,7 +8425,7 @@
       <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="205"/>
+      <c r="A29" s="207"/>
       <c r="B29" s="30" t="s">
         <v>134</v>
       </c>
@@ -8442,7 +8452,7 @@
       <c r="M29" s="35"/>
     </row>
     <row r="30" spans="1:13" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="204" t="s">
+      <c r="A30" s="206" t="s">
         <v>293</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -8475,7 +8485,7 @@
       <c r="M30" s="16"/>
     </row>
     <row r="31" spans="1:13" ht="40.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="204"/>
+      <c r="A31" s="206"/>
       <c r="B31" s="3" t="s">
         <v>111</v>
       </c>
@@ -8506,7 +8516,7 @@
       <c r="M31" s="16"/>
     </row>
     <row r="32" spans="1:13" s="29" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="205"/>
+      <c r="A32" s="207"/>
       <c r="B32" s="30" t="s">
         <v>134</v>
       </c>
@@ -8570,7 +8580,7 @@
       <c r="M33" s="50"/>
     </row>
     <row r="34" spans="1:13" s="44" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A34" s="203" t="s">
+      <c r="A34" s="205" t="s">
         <v>299</v>
       </c>
       <c r="B34" s="38" t="s">
@@ -8601,7 +8611,7 @@
       <c r="M34" s="43"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A35" s="204"/>
+      <c r="A35" s="206"/>
       <c r="B35" s="3" t="s">
         <v>141</v>
       </c>
@@ -8632,7 +8642,7 @@
       <c r="M35" s="16"/>
     </row>
     <row r="36" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A36" s="204"/>
+      <c r="A36" s="206"/>
       <c r="B36" s="3" t="s">
         <v>145</v>
       </c>
@@ -8661,7 +8671,7 @@
       <c r="M36" s="16"/>
     </row>
     <row r="37" spans="1:13" s="29" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A37" s="205"/>
+      <c r="A37" s="207"/>
       <c r="B37" s="30" t="s">
         <v>148</v>
       </c>
@@ -8690,7 +8700,7 @@
       <c r="M37" s="35"/>
     </row>
     <row r="38" spans="1:13" s="44" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A38" s="203" t="s">
+      <c r="A38" s="205" t="s">
         <v>286</v>
       </c>
       <c r="B38" s="38" t="s">
@@ -8723,7 +8733,7 @@
       <c r="M38" s="43"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A39" s="204"/>
+      <c r="A39" s="206"/>
       <c r="B39" s="3" t="s">
         <v>155</v>
       </c>
@@ -8754,7 +8764,7 @@
       <c r="M39" s="16"/>
     </row>
     <row r="40" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="204"/>
+      <c r="A40" s="206"/>
       <c r="B40" s="3" t="s">
         <v>158</v>
       </c>
@@ -8787,7 +8797,7 @@
       <c r="M40" s="16"/>
     </row>
     <row r="41" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A41" s="204"/>
+      <c r="A41" s="206"/>
       <c r="B41" s="3" t="s">
         <v>161</v>
       </c>
@@ -8820,7 +8830,7 @@
       <c r="M41" s="16"/>
     </row>
     <row r="42" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="204"/>
+      <c r="A42" s="206"/>
       <c r="B42" s="3" t="s">
         <v>165</v>
       </c>
@@ -8853,7 +8863,7 @@
       <c r="M42" s="16"/>
     </row>
     <row r="43" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="204"/>
+      <c r="A43" s="206"/>
       <c r="B43" s="3" t="s">
         <v>169</v>
       </c>
@@ -8884,7 +8894,7 @@
       <c r="M43" s="16"/>
     </row>
     <row r="44" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A44" s="204"/>
+      <c r="A44" s="206"/>
       <c r="B44" s="3" t="s">
         <v>172</v>
       </c>
@@ -8915,7 +8925,7 @@
       <c r="M44" s="16"/>
     </row>
     <row r="45" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="204"/>
+      <c r="A45" s="206"/>
       <c r="B45" s="3" t="s">
         <v>234</v>
       </c>
@@ -8944,7 +8954,7 @@
       <c r="M45" s="16"/>
     </row>
     <row r="46" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A46" s="204"/>
+      <c r="A46" s="206"/>
       <c r="B46" s="3" t="s">
         <v>237</v>
       </c>
@@ -8973,7 +8983,7 @@
       <c r="M46" s="16"/>
     </row>
     <row r="47" spans="1:13" s="29" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A47" s="205"/>
+      <c r="A47" s="207"/>
       <c r="B47" s="30" t="s">
         <v>240</v>
       </c>
@@ -9002,7 +9012,7 @@
       <c r="M47" s="35"/>
     </row>
     <row r="48" spans="1:13" s="44" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A48" s="203" t="s">
+      <c r="A48" s="205" t="s">
         <v>287</v>
       </c>
       <c r="B48" s="38" t="s">
@@ -9035,7 +9045,7 @@
       <c r="M48" s="43"/>
     </row>
     <row r="49" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A49" s="204"/>
+      <c r="A49" s="206"/>
       <c r="B49" s="3" t="s">
         <v>179</v>
       </c>
@@ -9066,7 +9076,7 @@
       <c r="M49" s="16"/>
     </row>
     <row r="50" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="204"/>
+      <c r="A50" s="206"/>
       <c r="B50" s="3" t="s">
         <v>183</v>
       </c>
@@ -9097,7 +9107,7 @@
       <c r="M50" s="16"/>
     </row>
     <row r="51" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="204"/>
+      <c r="A51" s="206"/>
       <c r="B51" s="3" t="s">
         <v>186</v>
       </c>
@@ -9126,7 +9136,7 @@
       <c r="M51" s="16"/>
     </row>
     <row r="52" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A52" s="204"/>
+      <c r="A52" s="206"/>
       <c r="B52" s="3" t="s">
         <v>189</v>
       </c>
@@ -9157,7 +9167,7 @@
       <c r="M52" s="16"/>
     </row>
     <row r="53" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A53" s="204"/>
+      <c r="A53" s="206"/>
       <c r="B53" s="3" t="s">
         <v>193</v>
       </c>
@@ -9188,7 +9198,7 @@
       <c r="M53" s="16"/>
     </row>
     <row r="54" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="204"/>
+      <c r="A54" s="206"/>
       <c r="B54" s="3" t="s">
         <v>196</v>
       </c>
@@ -9219,7 +9229,7 @@
       <c r="M54" s="16"/>
     </row>
     <row r="55" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A55" s="204"/>
+      <c r="A55" s="206"/>
       <c r="B55" s="3" t="s">
         <v>198</v>
       </c>
@@ -9250,7 +9260,7 @@
       <c r="M55" s="16"/>
     </row>
     <row r="56" spans="1:13" s="29" customFormat="1" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="205"/>
+      <c r="A56" s="207"/>
       <c r="B56" s="30" t="s">
         <v>205</v>
       </c>
@@ -9312,7 +9322,7 @@
       <c r="M57" s="50"/>
     </row>
     <row r="58" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A58" s="203" t="s">
+      <c r="A58" s="205" t="s">
         <v>290</v>
       </c>
       <c r="B58" s="3" t="s">
@@ -9347,7 +9357,7 @@
       </c>
     </row>
     <row r="59" spans="1:13" ht="57" x14ac:dyDescent="0.45">
-      <c r="A59" s="204"/>
+      <c r="A59" s="206"/>
       <c r="B59" s="3" t="s">
         <v>252</v>
       </c>
@@ -9380,7 +9390,7 @@
       </c>
     </row>
     <row r="60" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A60" s="204"/>
+      <c r="A60" s="206"/>
       <c r="B60" s="3" t="s">
         <v>255</v>
       </c>
@@ -9413,7 +9423,7 @@
       </c>
     </row>
     <row r="61" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A61" s="204"/>
+      <c r="A61" s="206"/>
       <c r="B61" s="3" t="s">
         <v>258</v>
       </c>
@@ -9446,7 +9456,7 @@
       </c>
     </row>
     <row r="62" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A62" s="204"/>
+      <c r="A62" s="206"/>
       <c r="B62" s="3" t="s">
         <v>261</v>
       </c>
@@ -9479,7 +9489,7 @@
       </c>
     </row>
     <row r="63" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A63" s="204"/>
+      <c r="A63" s="206"/>
       <c r="B63" s="3" t="s">
         <v>264</v>
       </c>
@@ -9512,7 +9522,7 @@
       </c>
     </row>
     <row r="64" spans="1:13" ht="57" x14ac:dyDescent="0.45">
-      <c r="A64" s="204"/>
+      <c r="A64" s="206"/>
       <c r="B64" s="3" t="s">
         <v>266</v>
       </c>
@@ -9545,7 +9555,7 @@
       </c>
     </row>
     <row r="65" spans="1:13" ht="57" x14ac:dyDescent="0.45">
-      <c r="A65" s="204"/>
+      <c r="A65" s="206"/>
       <c r="B65" s="3" t="s">
         <v>268</v>
       </c>
@@ -9578,7 +9588,7 @@
       </c>
     </row>
     <row r="66" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A66" s="204"/>
+      <c r="A66" s="206"/>
       <c r="B66" s="3" t="s">
         <v>270</v>
       </c>
@@ -9611,7 +9621,7 @@
       </c>
     </row>
     <row r="67" spans="1:13" s="29" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A67" s="205"/>
+      <c r="A67" s="207"/>
       <c r="B67" s="9" t="s">
         <v>272</v>
       </c>
@@ -9850,7 +9860,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="207" t="s">
+      <c r="A2" s="209" t="s">
         <v>423</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -9883,7 +9893,7 @@
       <c r="M2" s="16"/>
     </row>
     <row r="3" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="207"/>
+      <c r="A3" s="209"/>
       <c r="B3" s="3" t="s">
         <v>306</v>
       </c>
@@ -9912,7 +9922,7 @@
       <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="207"/>
+      <c r="A4" s="209"/>
       <c r="B4" s="3" t="s">
         <v>308</v>
       </c>
@@ -9941,7 +9951,7 @@
       <c r="M4" s="16"/>
     </row>
     <row r="5" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="207"/>
+      <c r="A5" s="209"/>
       <c r="B5" s="3" t="s">
         <v>319</v>
       </c>
@@ -9970,7 +9980,7 @@
       <c r="M5" s="16"/>
     </row>
     <row r="6" spans="1:13" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="207"/>
+      <c r="A6" s="209"/>
       <c r="B6" s="3" t="s">
         <v>324</v>
       </c>
@@ -10001,7 +10011,7 @@
       <c r="M6" s="16"/>
     </row>
     <row r="7" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="207"/>
+      <c r="A7" s="209"/>
       <c r="B7" s="3" t="s">
         <v>402</v>
       </c>
@@ -10032,7 +10042,7 @@
       <c r="M7" s="16"/>
     </row>
     <row r="8" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="207"/>
+      <c r="A8" s="209"/>
       <c r="B8" s="3" t="s">
         <v>406</v>
       </c>
@@ -10061,7 +10071,7 @@
       <c r="M8" s="16"/>
     </row>
     <row r="9" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="207"/>
+      <c r="A9" s="209"/>
       <c r="B9" s="3" t="s">
         <v>413</v>
       </c>
@@ -10090,7 +10100,7 @@
       <c r="M9" s="16"/>
     </row>
     <row r="10" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="207"/>
+      <c r="A10" s="209"/>
       <c r="B10" s="3" t="s">
         <v>415</v>
       </c>
@@ -10119,7 +10129,7 @@
       <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="207"/>
+      <c r="A11" s="209"/>
       <c r="B11" s="3" t="s">
         <v>419</v>
       </c>
@@ -10148,7 +10158,7 @@
       <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="208"/>
+      <c r="A12" s="210"/>
       <c r="B12" s="3" t="s">
         <v>421</v>
       </c>
@@ -10177,7 +10187,7 @@
       <c r="M12" s="16"/>
     </row>
     <row r="13" spans="1:13" s="38" customFormat="1" ht="27.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="206" t="s">
+      <c r="A13" s="208" t="s">
         <v>424</v>
       </c>
       <c r="B13" s="38" t="s">
@@ -10210,7 +10220,7 @@
       <c r="M13" s="43"/>
     </row>
     <row r="14" spans="1:13" s="3" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="208"/>
+      <c r="A14" s="210"/>
       <c r="B14" s="3" t="s">
         <v>336</v>
       </c>
@@ -10241,7 +10251,7 @@
       <c r="M14" s="16"/>
     </row>
     <row r="15" spans="1:13" s="38" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="206" t="s">
+      <c r="A15" s="208" t="s">
         <v>425</v>
       </c>
       <c r="B15" s="38" t="s">
@@ -10274,7 +10284,7 @@
       <c r="M15" s="43"/>
     </row>
     <row r="16" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="207"/>
+      <c r="A16" s="209"/>
       <c r="B16" s="3" t="s">
         <v>322</v>
       </c>
@@ -10305,7 +10315,7 @@
       <c r="M16" s="16"/>
     </row>
     <row r="17" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="207"/>
+      <c r="A17" s="209"/>
       <c r="B17" s="3" t="s">
         <v>379</v>
       </c>
@@ -10336,7 +10346,7 @@
       <c r="M17" s="16"/>
     </row>
     <row r="18" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="207"/>
+      <c r="A18" s="209"/>
       <c r="B18" s="3" t="s">
         <v>389</v>
       </c>
@@ -10367,7 +10377,7 @@
       <c r="M18" s="16"/>
     </row>
     <row r="19" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="207"/>
+      <c r="A19" s="209"/>
       <c r="B19" s="3" t="s">
         <v>392</v>
       </c>
@@ -10398,7 +10408,7 @@
       <c r="M19" s="16"/>
     </row>
     <row r="20" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="207"/>
+      <c r="A20" s="209"/>
       <c r="B20" s="3" t="s">
         <v>396</v>
       </c>
@@ -10427,7 +10437,7 @@
       <c r="M20" s="16"/>
     </row>
     <row r="21" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="208"/>
+      <c r="A21" s="210"/>
       <c r="B21" s="3" t="s">
         <v>409</v>
       </c>
@@ -10458,7 +10468,7 @@
       <c r="M21" s="16"/>
     </row>
     <row r="22" spans="1:13" s="38" customFormat="1" ht="28.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="206" t="s">
+      <c r="A22" s="208" t="s">
         <v>426</v>
       </c>
       <c r="B22" s="38" t="s">
@@ -10491,7 +10501,7 @@
       <c r="M22" s="43"/>
     </row>
     <row r="23" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="207"/>
+      <c r="A23" s="209"/>
       <c r="B23" s="3" t="s">
         <v>386</v>
       </c>
@@ -10522,7 +10532,7 @@
       <c r="M23" s="16"/>
     </row>
     <row r="24" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="208"/>
+      <c r="A24" s="210"/>
       <c r="B24" s="3" t="s">
         <v>389</v>
       </c>
@@ -10553,7 +10563,7 @@
       <c r="M24" s="16"/>
     </row>
     <row r="25" spans="1:13" s="38" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="209" t="s">
+      <c r="A25" s="211" t="s">
         <v>294</v>
       </c>
       <c r="B25" s="38" t="s">
@@ -10586,7 +10596,7 @@
       <c r="M25" s="42"/>
     </row>
     <row r="26" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="210"/>
+      <c r="A26" s="212"/>
       <c r="B26" s="3" t="s">
         <v>329</v>
       </c>
@@ -10617,7 +10627,7 @@
       <c r="M26" s="18"/>
     </row>
     <row r="27" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="210"/>
+      <c r="A27" s="212"/>
       <c r="B27" s="3" t="s">
         <v>335</v>
       </c>
@@ -10648,7 +10658,7 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="210"/>
+      <c r="A28" s="212"/>
       <c r="B28" s="3" t="s">
         <v>339</v>
       </c>
@@ -10681,7 +10691,7 @@
       <c r="M28" s="16"/>
     </row>
     <row r="29" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="210"/>
+      <c r="A29" s="212"/>
       <c r="B29" s="3" t="s">
         <v>340</v>
       </c>
@@ -10712,7 +10722,7 @@
       <c r="M29" s="16"/>
     </row>
     <row r="30" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="211"/>
+      <c r="A30" s="213"/>
       <c r="B30" s="3" t="s">
         <v>411</v>
       </c>
@@ -10743,7 +10753,7 @@
       <c r="M30" s="70"/>
     </row>
     <row r="31" spans="1:13" s="38" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="206" t="s">
+      <c r="A31" s="208" t="s">
         <v>427</v>
       </c>
       <c r="B31" s="38" t="s">
@@ -10776,7 +10786,7 @@
       <c r="M31" s="42"/>
     </row>
     <row r="32" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="207"/>
+      <c r="A32" s="209"/>
       <c r="B32" s="3" t="s">
         <v>343</v>
       </c>
@@ -10807,7 +10817,7 @@
       <c r="M32" s="16"/>
     </row>
     <row r="33" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="207"/>
+      <c r="A33" s="209"/>
       <c r="B33" s="3" t="s">
         <v>346</v>
       </c>
@@ -10838,7 +10848,7 @@
       <c r="M33" s="16"/>
     </row>
     <row r="34" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="207"/>
+      <c r="A34" s="209"/>
       <c r="B34" s="3" t="s">
         <v>348</v>
       </c>
@@ -10871,7 +10881,7 @@
       <c r="M34" s="16"/>
     </row>
     <row r="35" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A35" s="207"/>
+      <c r="A35" s="209"/>
       <c r="B35" s="3" t="s">
         <v>349</v>
       </c>
@@ -10904,7 +10914,7 @@
       <c r="M35" s="16"/>
     </row>
     <row r="36" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A36" s="207"/>
+      <c r="A36" s="209"/>
       <c r="B36" s="3" t="s">
         <v>352</v>
       </c>
@@ -10937,7 +10947,7 @@
       <c r="M36" s="16"/>
     </row>
     <row r="37" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="207"/>
+      <c r="A37" s="209"/>
       <c r="B37" s="3" t="s">
         <v>353</v>
       </c>
@@ -10968,7 +10978,7 @@
       <c r="M37" s="16"/>
     </row>
     <row r="38" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A38" s="207"/>
+      <c r="A38" s="209"/>
       <c r="B38" s="3" t="s">
         <v>356</v>
       </c>
@@ -10999,7 +11009,7 @@
       <c r="M38" s="16"/>
     </row>
     <row r="39" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="208"/>
+      <c r="A39" s="210"/>
       <c r="B39" s="3" t="s">
         <v>358</v>
       </c>
@@ -11063,7 +11073,7 @@
       <c r="M40" s="43"/>
     </row>
     <row r="41" spans="1:13" s="38" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="206" t="s">
+      <c r="A41" s="208" t="s">
         <v>429</v>
       </c>
       <c r="B41" s="38" t="s">
@@ -11096,7 +11106,7 @@
       <c r="M41" s="43"/>
     </row>
     <row r="42" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A42" s="207"/>
+      <c r="A42" s="209"/>
       <c r="B42" s="3" t="s">
         <v>384</v>
       </c>
@@ -11125,7 +11135,7 @@
       <c r="M42" s="16"/>
     </row>
     <row r="43" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A43" s="207"/>
+      <c r="A43" s="209"/>
       <c r="B43" s="3" t="s">
         <v>389</v>
       </c>
@@ -11156,7 +11166,7 @@
       <c r="M43" s="16"/>
     </row>
     <row r="44" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="208"/>
+      <c r="A44" s="210"/>
       <c r="B44" s="3" t="s">
         <v>399</v>
       </c>
@@ -11185,7 +11195,7 @@
       <c r="M44" s="16"/>
     </row>
     <row r="45" spans="1:13" s="38" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A45" s="206" t="s">
+      <c r="A45" s="208" t="s">
         <v>430</v>
       </c>
       <c r="B45" s="38" t="s">
@@ -11218,7 +11228,7 @@
       <c r="M45" s="43"/>
     </row>
     <row r="46" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A46" s="207"/>
+      <c r="A46" s="209"/>
       <c r="B46" s="3" t="s">
         <v>369</v>
       </c>
@@ -11247,7 +11257,7 @@
       <c r="M46" s="16"/>
     </row>
     <row r="47" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A47" s="207"/>
+      <c r="A47" s="209"/>
       <c r="B47" s="3" t="s">
         <v>371</v>
       </c>
@@ -11278,7 +11288,7 @@
       <c r="M47" s="16"/>
     </row>
     <row r="48" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A48" s="207"/>
+      <c r="A48" s="209"/>
       <c r="B48" s="3" t="s">
         <v>373</v>
       </c>
@@ -11309,7 +11319,7 @@
       <c r="M48" s="16"/>
     </row>
     <row r="49" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A49" s="207"/>
+      <c r="A49" s="209"/>
       <c r="B49" s="3" t="s">
         <v>376</v>
       </c>
@@ -11340,7 +11350,7 @@
       <c r="M49" s="16"/>
     </row>
     <row r="50" spans="1:13" s="3" customFormat="1" ht="14.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="207"/>
+      <c r="A50" s="209"/>
       <c r="B50" s="3" t="s">
         <v>378</v>
       </c>
@@ -11545,7 +11555,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A2" s="212" t="s">
+      <c r="A2" s="214" t="s">
         <v>531</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -11578,7 +11588,7 @@
       <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="213"/>
+      <c r="A3" s="215"/>
       <c r="B3" s="3" t="s">
         <v>490</v>
       </c>
@@ -11609,7 +11619,7 @@
       <c r="M3" s="18"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="213"/>
+      <c r="A4" s="215"/>
       <c r="B4" s="3" t="s">
         <v>491</v>
       </c>
@@ -11640,7 +11650,7 @@
       <c r="M4" s="18"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="213"/>
+      <c r="A5" s="215"/>
       <c r="B5" s="3" t="s">
         <v>494</v>
       </c>
@@ -11669,7 +11679,7 @@
       <c r="M5" s="18"/>
     </row>
     <row r="6" spans="1:13" ht="29.35" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="213"/>
+      <c r="A6" s="215"/>
       <c r="B6" s="3" t="s">
         <v>495</v>
       </c>
@@ -11698,7 +11708,7 @@
       <c r="M6" s="18"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="213"/>
+      <c r="A7" s="215"/>
       <c r="B7" s="3" t="s">
         <v>496</v>
       </c>
@@ -11729,7 +11739,7 @@
       <c r="M7" s="18"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="214"/>
+      <c r="A8" s="216"/>
       <c r="B8" s="3" t="s">
         <v>530</v>
       </c>
@@ -11758,7 +11768,7 @@
       <c r="M8" s="18"/>
     </row>
     <row r="9" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="212" t="s">
+      <c r="A9" s="214" t="s">
         <v>537</v>
       </c>
       <c r="B9" s="38" t="s">
@@ -11791,7 +11801,7 @@
       <c r="M9" s="42"/>
     </row>
     <row r="10" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="213"/>
+      <c r="A10" s="215"/>
       <c r="B10" s="3" t="s">
         <v>519</v>
       </c>
@@ -11822,7 +11832,7 @@
       <c r="M10" s="18"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="213"/>
+      <c r="A11" s="215"/>
       <c r="B11" s="3" t="s">
         <v>522</v>
       </c>
@@ -11853,7 +11863,7 @@
       <c r="M11" s="18"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="213"/>
+      <c r="A12" s="215"/>
       <c r="B12" s="3" t="s">
         <v>523</v>
       </c>
@@ -11884,7 +11894,7 @@
       <c r="M12" s="18"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A13" s="213"/>
+      <c r="A13" s="215"/>
       <c r="B13" s="3" t="s">
         <v>524</v>
       </c>
@@ -11913,7 +11923,7 @@
       <c r="M13" s="18"/>
     </row>
     <row r="14" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="213"/>
+      <c r="A14" s="215"/>
       <c r="B14" s="3" t="s">
         <v>526</v>
       </c>
@@ -11944,7 +11954,7 @@
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" s="214"/>
+      <c r="A15" s="216"/>
       <c r="B15" s="3" t="s">
         <v>528</v>
       </c>
@@ -11975,7 +11985,7 @@
       <c r="M15" s="18"/>
     </row>
     <row r="16" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="212" t="s">
+      <c r="A16" s="214" t="s">
         <v>538</v>
       </c>
       <c r="B16" s="38" t="s">
@@ -12008,7 +12018,7 @@
       <c r="M16" s="42"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="213"/>
+      <c r="A17" s="215"/>
       <c r="B17" s="3" t="s">
         <v>521</v>
       </c>
@@ -12039,7 +12049,7 @@
       <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="213"/>
+      <c r="A18" s="215"/>
       <c r="B18" s="3" t="s">
         <v>522</v>
       </c>
@@ -12070,7 +12080,7 @@
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="214"/>
+      <c r="A19" s="216"/>
       <c r="B19" s="3" t="s">
         <v>527</v>
       </c>
@@ -12099,7 +12109,7 @@
       <c r="M19" s="18"/>
     </row>
     <row r="20" spans="1:13" s="44" customFormat="1" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="212" t="s">
+      <c r="A20" s="214" t="s">
         <v>532</v>
       </c>
       <c r="B20" s="38" t="s">
@@ -12130,7 +12140,7 @@
       <c r="M20" s="42"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="213"/>
+      <c r="A21" s="215"/>
       <c r="B21" s="3" t="s">
         <v>499</v>
       </c>
@@ -12161,7 +12171,7 @@
       <c r="M21" s="18"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="214"/>
+      <c r="A22" s="216"/>
       <c r="B22" s="3" t="s">
         <v>510</v>
       </c>
@@ -12194,7 +12204,7 @@
       <c r="M22" s="16"/>
     </row>
     <row r="23" spans="1:13" s="44" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="212" t="s">
+      <c r="A23" s="214" t="s">
         <v>294</v>
       </c>
       <c r="B23" s="38" t="s">
@@ -12227,7 +12237,7 @@
       <c r="M23" s="42"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="213"/>
+      <c r="A24" s="215"/>
       <c r="B24" s="3" t="s">
         <v>499</v>
       </c>
@@ -12258,7 +12268,7 @@
       <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="214"/>
+      <c r="A25" s="216"/>
       <c r="B25" s="3" t="s">
         <v>529</v>
       </c>
@@ -12289,7 +12299,7 @@
       <c r="M25" s="17"/>
     </row>
     <row r="26" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="212" t="s">
+      <c r="A26" s="214" t="s">
         <v>533</v>
       </c>
       <c r="B26" s="38" t="s">
@@ -12322,7 +12332,7 @@
       <c r="M26" s="42"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A27" s="213"/>
+      <c r="A27" s="215"/>
       <c r="B27" s="3" t="s">
         <v>504</v>
       </c>
@@ -12353,7 +12363,7 @@
       <c r="M27" s="18"/>
     </row>
     <row r="28" spans="1:13" ht="38.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="213"/>
+      <c r="A28" s="215"/>
       <c r="B28" s="3" t="s">
         <v>505</v>
       </c>
@@ -12384,7 +12394,7 @@
       <c r="M28" s="18"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A29" s="213"/>
+      <c r="A29" s="215"/>
       <c r="B29" s="3" t="s">
         <v>506</v>
       </c>
@@ -12417,7 +12427,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="213"/>
+      <c r="A30" s="215"/>
       <c r="B30" s="3" t="s">
         <v>507</v>
       </c>
@@ -12450,7 +12460,7 @@
       <c r="M30" s="18"/>
     </row>
     <row r="31" spans="1:13" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="213"/>
+      <c r="A31" s="215"/>
       <c r="B31" s="3" t="s">
         <v>508</v>
       </c>
@@ -12481,7 +12491,7 @@
       <c r="M31" s="18"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A32" s="213"/>
+      <c r="A32" s="215"/>
       <c r="B32" s="3" t="s">
         <v>511</v>
       </c>
@@ -12512,7 +12522,7 @@
       <c r="M32" s="16"/>
     </row>
     <row r="33" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="214"/>
+      <c r="A33" s="216"/>
       <c r="B33" s="30" t="s">
         <v>509</v>
       </c>
@@ -12543,7 +12553,7 @@
       <c r="M33" s="34"/>
     </row>
     <row r="34" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="212" t="s">
+      <c r="A34" s="214" t="s">
         <v>534</v>
       </c>
       <c r="B34" s="38" t="s">
@@ -12576,7 +12586,7 @@
       <c r="M34" s="42"/>
     </row>
     <row r="35" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="213"/>
+      <c r="A35" s="215"/>
       <c r="B35" s="3" t="s">
         <v>512</v>
       </c>
@@ -12607,7 +12617,7 @@
       <c r="M35" s="18"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A36" s="213"/>
+      <c r="A36" s="215"/>
       <c r="B36" s="3" t="s">
         <v>520</v>
       </c>
@@ -12636,7 +12646,7 @@
       <c r="M36" s="18"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A37" s="213"/>
+      <c r="A37" s="215"/>
       <c r="B37" s="3" t="s">
         <v>522</v>
       </c>
@@ -12667,7 +12677,7 @@
       <c r="M37" s="18"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A38" s="214"/>
+      <c r="A38" s="216"/>
       <c r="B38" s="3" t="s">
         <v>525</v>
       </c>
@@ -12696,7 +12706,7 @@
       <c r="M38" s="18"/>
     </row>
     <row r="39" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="212" t="s">
+      <c r="A39" s="214" t="s">
         <v>535</v>
       </c>
       <c r="B39" s="38" t="s">
@@ -12731,7 +12741,7 @@
       <c r="M39" s="42"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A40" s="214"/>
+      <c r="A40" s="216"/>
       <c r="B40" s="3" t="s">
         <v>503</v>
       </c>
@@ -12762,7 +12772,7 @@
       <c r="M40" s="18"/>
     </row>
     <row r="41" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="212" t="s">
+      <c r="A41" s="214" t="s">
         <v>536</v>
       </c>
       <c r="B41" s="38" t="s">
@@ -12795,7 +12805,7 @@
       <c r="M41" s="42"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A42" s="213"/>
+      <c r="A42" s="215"/>
       <c r="B42" s="3" t="s">
         <v>514</v>
       </c>
@@ -12824,7 +12834,7 @@
       <c r="M42" s="18"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A43" s="213"/>
+      <c r="A43" s="215"/>
       <c r="B43" s="3" t="s">
         <v>515</v>
       </c>
@@ -12855,7 +12865,7 @@
       <c r="M43" s="18"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A44" s="213"/>
+      <c r="A44" s="215"/>
       <c r="B44" s="3" t="s">
         <v>516</v>
       </c>
@@ -12886,7 +12896,7 @@
       <c r="M44" s="18"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A45" s="213"/>
+      <c r="A45" s="215"/>
       <c r="B45" s="3" t="s">
         <v>517</v>
       </c>
@@ -12915,7 +12925,7 @@
       <c r="M45" s="18"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A46" s="214"/>
+      <c r="A46" s="216"/>
       <c r="B46" s="3" t="s">
         <v>518</v>
       </c>
@@ -13140,7 +13150,7 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="204" t="s">
+      <c r="A2" s="206" t="s">
         <v>531</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -13172,7 +13182,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A3" s="204"/>
+      <c r="A3" s="206"/>
       <c r="B3" s="3" t="s">
         <v>543</v>
       </c>
@@ -13200,7 +13210,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A4" s="204"/>
+      <c r="A4" s="206"/>
       <c r="B4" s="3" t="s">
         <v>545</v>
       </c>
@@ -13228,7 +13238,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A5" s="204"/>
+      <c r="A5" s="206"/>
       <c r="B5" s="3" t="s">
         <v>552</v>
       </c>
@@ -13256,7 +13266,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A6" s="204"/>
+      <c r="A6" s="206"/>
       <c r="B6" s="3" t="s">
         <v>556</v>
       </c>
@@ -13286,7 +13296,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A7" s="204"/>
+      <c r="A7" s="206"/>
       <c r="B7" s="3" t="s">
         <v>558</v>
       </c>
@@ -13314,7 +13324,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A8" s="204"/>
+      <c r="A8" s="206"/>
       <c r="B8" s="3" t="s">
         <v>605</v>
       </c>
@@ -13344,7 +13354,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="204"/>
+      <c r="A9" s="206"/>
       <c r="B9" s="3" t="s">
         <v>616</v>
       </c>
@@ -13374,7 +13384,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="204"/>
+      <c r="A10" s="206"/>
       <c r="B10" s="3" t="s">
         <v>627</v>
       </c>
@@ -13404,7 +13414,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A11" s="204"/>
+      <c r="A11" s="206"/>
       <c r="B11" s="3" t="s">
         <v>630</v>
       </c>
@@ -13432,7 +13442,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A12" s="205"/>
+      <c r="A12" s="207"/>
       <c r="B12" s="3" t="s">
         <v>636</v>
       </c>
@@ -13460,7 +13470,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="203" t="s">
+      <c r="A13" s="205" t="s">
         <v>537</v>
       </c>
       <c r="B13" s="38" t="s">
@@ -13492,7 +13502,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A14" s="204"/>
+      <c r="A14" s="206"/>
       <c r="B14" s="3" t="s">
         <v>554</v>
       </c>
@@ -13522,7 +13532,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A15" s="204"/>
+      <c r="A15" s="206"/>
       <c r="B15" s="3" t="s">
         <v>620</v>
       </c>
@@ -13552,7 +13562,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A16" s="204"/>
+      <c r="A16" s="206"/>
       <c r="B16" s="3" t="s">
         <v>623</v>
       </c>
@@ -13580,7 +13590,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="205"/>
+      <c r="A17" s="207"/>
       <c r="B17" s="3" t="s">
         <v>632</v>
       </c>
@@ -13610,7 +13620,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="203" t="s">
+      <c r="A18" s="205" t="s">
         <v>538</v>
       </c>
       <c r="B18" s="38" t="s">
@@ -13642,7 +13652,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="204"/>
+      <c r="A19" s="206"/>
       <c r="B19" s="3" t="s">
         <v>612</v>
       </c>
@@ -13672,7 +13682,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="205"/>
+      <c r="A20" s="207"/>
       <c r="B20" s="3" t="s">
         <v>616</v>
       </c>
@@ -13702,7 +13712,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" s="44" customFormat="1" ht="51.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="203" t="s">
+      <c r="A21" s="205" t="s">
         <v>294</v>
       </c>
       <c r="B21" s="38" t="s">
@@ -13734,7 +13744,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="204"/>
+      <c r="A22" s="206"/>
       <c r="B22" s="3" t="s">
         <v>563</v>
       </c>
@@ -13764,7 +13774,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="204"/>
+      <c r="A23" s="206"/>
       <c r="B23" s="3" t="s">
         <v>568</v>
       </c>
@@ -13796,7 +13806,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="204"/>
+      <c r="A24" s="206"/>
       <c r="B24" s="3" t="s">
         <v>570</v>
       </c>
@@ -13826,7 +13836,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="205"/>
+      <c r="A25" s="207"/>
       <c r="B25" s="3" t="s">
         <v>634</v>
       </c>
@@ -13856,7 +13866,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="203" t="s">
+      <c r="A26" s="205" t="s">
         <v>637</v>
       </c>
       <c r="B26" s="38" t="s">
@@ -13888,7 +13898,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="204"/>
+      <c r="A27" s="206"/>
       <c r="B27" s="3" t="s">
         <v>572</v>
       </c>
@@ -13918,7 +13928,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="54.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="204"/>
+      <c r="A28" s="206"/>
       <c r="B28" s="3" t="s">
         <v>576</v>
       </c>
@@ -13950,7 +13960,7 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A29" s="204"/>
+      <c r="A29" s="206"/>
       <c r="B29" s="3" t="s">
         <v>579</v>
       </c>
@@ -13982,7 +13992,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="204"/>
+      <c r="A30" s="206"/>
       <c r="B30" s="3" t="s">
         <v>580</v>
       </c>
@@ -14014,7 +14024,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="204"/>
+      <c r="A31" s="206"/>
       <c r="B31" s="3" t="s">
         <v>582</v>
       </c>
@@ -14044,7 +14054,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="204"/>
+      <c r="A32" s="206"/>
       <c r="B32" s="3" t="s">
         <v>585</v>
       </c>
@@ -14074,7 +14084,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="205"/>
+      <c r="A33" s="207"/>
       <c r="B33" s="3" t="s">
         <v>587</v>
       </c>
@@ -14104,7 +14114,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="203" t="s">
+      <c r="A34" s="205" t="s">
         <v>638</v>
       </c>
       <c r="B34" s="38" t="s">
@@ -14136,7 +14146,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" s="204"/>
+      <c r="A35" s="206"/>
       <c r="B35" s="3" t="s">
         <v>589</v>
       </c>
@@ -14166,7 +14176,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" s="204"/>
+      <c r="A36" s="206"/>
       <c r="B36" s="3" t="s">
         <v>609</v>
       </c>
@@ -14194,7 +14204,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="204"/>
+      <c r="A37" s="206"/>
       <c r="B37" s="3" t="s">
         <v>616</v>
       </c>
@@ -14224,7 +14234,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A38" s="205"/>
+      <c r="A38" s="207"/>
       <c r="B38" s="3" t="s">
         <v>625</v>
       </c>
@@ -14252,7 +14262,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A39" s="203" t="s">
+      <c r="A39" s="205" t="s">
         <v>536</v>
       </c>
       <c r="B39" s="38" t="s">
@@ -14284,7 +14294,7 @@
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A40" s="204"/>
+      <c r="A40" s="206"/>
       <c r="B40" s="3" t="s">
         <v>596</v>
       </c>
@@ -14312,7 +14322,7 @@
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A41" s="204"/>
+      <c r="A41" s="206"/>
       <c r="B41" s="3" t="s">
         <v>598</v>
       </c>
@@ -14342,7 +14352,7 @@
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A42" s="204"/>
+      <c r="A42" s="206"/>
       <c r="B42" s="3" t="s">
         <v>601</v>
       </c>
@@ -14372,7 +14382,7 @@
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A43" s="204"/>
+      <c r="A43" s="206"/>
       <c r="B43" s="3" t="s">
         <v>603</v>
       </c>
@@ -14400,7 +14410,7 @@
       </c>
     </row>
     <row r="44" spans="1:12" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A44" s="205"/>
+      <c r="A44" s="207"/>
       <c r="B44" s="30" t="s">
         <v>604</v>
       </c>

</xml_diff>